<commit_message>
add: harga-sewa-create; update: tb_rkap, tb_rkap_detail;
</commit_message>
<xml_diff>
--- a/database/seeds/rkap.xlsx
+++ b/database/seeds/rkap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>kd_rkap</t>
   </si>
@@ -78,6 +78,33 @@
   </si>
   <si>
     <t>R20201000008</t>
+  </si>
+  <si>
+    <t>Suku Cadang</t>
+  </si>
+  <si>
+    <t>Bahan Pembantu</t>
+  </si>
+  <si>
+    <t>Pemeliharaan - Kendaraan</t>
+  </si>
+  <si>
+    <t>Pajak Kendaraan</t>
+  </si>
+  <si>
+    <t>Retribusi - Kendaraan</t>
+  </si>
+  <si>
+    <t>Sewa - Kendaraan</t>
+  </si>
+  <si>
+    <t>Lainnya - Bahan Bakar Kendaraan</t>
+  </si>
+  <si>
+    <t>Retribusi - Parkir &amp; Tol</t>
+  </si>
+  <si>
+    <t>uraian</t>
   </si>
 </sst>
 </file>
@@ -438,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,10 +476,11 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,19 +491,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -485,20 +516,23 @@
       <c r="C2">
         <v>630110000</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
         <v>2020</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>301000000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -508,20 +542,23 @@
       <c r="C3">
         <v>610220000</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
         <v>2020</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>51329267</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -531,20 +568,23 @@
       <c r="C4">
         <v>690110010</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4">
         <v>2020</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>4664101320</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -554,20 +594,23 @@
       <c r="C5">
         <v>630210008</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
         <v>2020</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1107774718</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -577,20 +620,23 @@
       <c r="C6">
         <v>640210002</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
         <v>2020</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>274294680</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -600,20 +646,23 @@
       <c r="C7">
         <v>640220003</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
         <v>2020</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>19216020</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -623,20 +672,23 @@
       <c r="C8">
         <v>640220006</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
         <v>2020</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>216000000</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -646,16 +698,19 @@
       <c r="C9">
         <v>670220001</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9">
         <v>2020</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>21780569455</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>